<commit_message>
added enable/disable visit button
</commit_message>
<xml_diff>
--- a/Governance-App/uploads/ecommerce.xlsx
+++ b/Governance-App/uploads/ecommerce.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="129">
   <si>
     <t>_sa_instance_state</t>
   </si>
@@ -28,199 +28,205 @@
     <t>userName</t>
   </si>
   <si>
+    <t>auditModuleName</t>
+  </si>
+  <si>
+    <t>auditid</t>
+  </si>
+  <si>
     <t>operation</t>
   </si>
   <si>
-    <t>auditModuleName</t>
-  </si>
-  <si>
-    <t>auditid</t>
-  </si>
-  <si>
     <t>timestamp</t>
   </si>
   <si>
-    <t>&lt;sqlalchemy.orm.state.InstanceState object at 0x7f05504e65b0&gt;</t>
-  </si>
-  <si>
-    <t>&lt;sqlalchemy.orm.state.InstanceState object at 0x7f05504e65e0&gt;</t>
-  </si>
-  <si>
-    <t>&lt;sqlalchemy.orm.state.InstanceState object at 0x7f05504e6640&gt;</t>
-  </si>
-  <si>
-    <t>&lt;sqlalchemy.orm.state.InstanceState object at 0x7f05504e66a0&gt;</t>
-  </si>
-  <si>
-    <t>&lt;sqlalchemy.orm.state.InstanceState object at 0x7f05504e6700&gt;</t>
-  </si>
-  <si>
-    <t>&lt;sqlalchemy.orm.state.InstanceState object at 0x7f05504e6760&gt;</t>
-  </si>
-  <si>
-    <t>&lt;sqlalchemy.orm.state.InstanceState object at 0x7f05504e67c0&gt;</t>
-  </si>
-  <si>
-    <t>&lt;sqlalchemy.orm.state.InstanceState object at 0x7f05504e6820&gt;</t>
-  </si>
-  <si>
-    <t>&lt;sqlalchemy.orm.state.InstanceState object at 0x7f05504e6880&gt;</t>
-  </si>
-  <si>
-    <t>&lt;sqlalchemy.orm.state.InstanceState object at 0x7f05504e68e0&gt;</t>
-  </si>
-  <si>
-    <t>&lt;sqlalchemy.orm.state.InstanceState object at 0x7f05504e6940&gt;</t>
-  </si>
-  <si>
-    <t>&lt;sqlalchemy.orm.state.InstanceState object at 0x7f05504e69a0&gt;</t>
-  </si>
-  <si>
-    <t>&lt;sqlalchemy.orm.state.InstanceState object at 0x7f05504e6a00&gt;</t>
-  </si>
-  <si>
-    <t>&lt;sqlalchemy.orm.state.InstanceState object at 0x7f05504e6a60&gt;</t>
-  </si>
-  <si>
-    <t>&lt;sqlalchemy.orm.state.InstanceState object at 0x7f05504e6ac0&gt;</t>
-  </si>
-  <si>
-    <t>&lt;sqlalchemy.orm.state.InstanceState object at 0x7f05504e6b20&gt;</t>
-  </si>
-  <si>
-    <t>&lt;sqlalchemy.orm.state.InstanceState object at 0x7f05504e6b80&gt;</t>
-  </si>
-  <si>
-    <t>&lt;sqlalchemy.orm.state.InstanceState object at 0x7f05504e6be0&gt;</t>
-  </si>
-  <si>
-    <t>&lt;sqlalchemy.orm.state.InstanceState object at 0x7f05504e6c40&gt;</t>
-  </si>
-  <si>
-    <t>&lt;sqlalchemy.orm.state.InstanceState object at 0x7f05504e6ca0&gt;</t>
-  </si>
-  <si>
-    <t>&lt;sqlalchemy.orm.state.InstanceState object at 0x7f05504e6d00&gt;</t>
-  </si>
-  <si>
-    <t>&lt;sqlalchemy.orm.state.InstanceState object at 0x7f05504e6d60&gt;</t>
-  </si>
-  <si>
-    <t>&lt;sqlalchemy.orm.state.InstanceState object at 0x7f05504e6dc0&gt;</t>
-  </si>
-  <si>
-    <t>&lt;sqlalchemy.orm.state.InstanceState object at 0x7f05504e6e20&gt;</t>
-  </si>
-  <si>
-    <t>&lt;sqlalchemy.orm.state.InstanceState object at 0x7f05504e6e80&gt;</t>
-  </si>
-  <si>
-    <t>&lt;sqlalchemy.orm.state.InstanceState object at 0x7f05504e6ee0&gt;</t>
-  </si>
-  <si>
-    <t>&lt;sqlalchemy.orm.state.InstanceState object at 0x7f05504e6f40&gt;</t>
-  </si>
-  <si>
-    <t>&lt;sqlalchemy.orm.state.InstanceState object at 0x7f05504e6fa0&gt;</t>
-  </si>
-  <si>
-    <t>&lt;sqlalchemy.orm.state.InstanceState object at 0x7f05504e2040&gt;</t>
-  </si>
-  <si>
-    <t>&lt;sqlalchemy.orm.state.InstanceState object at 0x7f05504e20a0&gt;</t>
-  </si>
-  <si>
-    <t>&lt;sqlalchemy.orm.state.InstanceState object at 0x7f05504e2100&gt;</t>
-  </si>
-  <si>
-    <t>&lt;sqlalchemy.orm.state.InstanceState object at 0x7f05504e2160&gt;</t>
-  </si>
-  <si>
-    <t>&lt;sqlalchemy.orm.state.InstanceState object at 0x7f0570f42c10&gt;</t>
-  </si>
-  <si>
-    <t>&lt;sqlalchemy.orm.state.InstanceState object at 0x7f0570f42af0&gt;</t>
-  </si>
-  <si>
-    <t>&lt;sqlalchemy.orm.state.InstanceState object at 0x7f05530fae80&gt;</t>
-  </si>
-  <si>
-    <t>&lt;sqlalchemy.orm.state.InstanceState object at 0x7f05530fafa0&gt;</t>
-  </si>
-  <si>
-    <t>&lt;sqlalchemy.orm.state.InstanceState object at 0x7f0570eb8910&gt;</t>
-  </si>
-  <si>
-    <t>&lt;sqlalchemy.orm.state.InstanceState object at 0x7f0570eb8580&gt;</t>
-  </si>
-  <si>
-    <t>&lt;sqlalchemy.orm.state.InstanceState object at 0x7f0551fd9850&gt;</t>
-  </si>
-  <si>
-    <t>&lt;sqlalchemy.orm.state.InstanceState object at 0x7f0551fd9220&gt;</t>
-  </si>
-  <si>
-    <t>&lt;sqlalchemy.orm.state.InstanceState object at 0x7f0551fd9610&gt;</t>
-  </si>
-  <si>
-    <t>&lt;sqlalchemy.orm.state.InstanceState object at 0x7f0551fd94f0&gt;</t>
-  </si>
-  <si>
-    <t>&lt;sqlalchemy.orm.state.InstanceState object at 0x7f0551fd91f0&gt;</t>
-  </si>
-  <si>
-    <t>&lt;sqlalchemy.orm.state.InstanceState object at 0x7f0551fd9550&gt;</t>
-  </si>
-  <si>
-    <t>&lt;sqlalchemy.orm.state.InstanceState object at 0x7f0570ea1f40&gt;</t>
-  </si>
-  <si>
-    <t>&lt;sqlalchemy.orm.state.InstanceState object at 0x7f0570ea1520&gt;</t>
-  </si>
-  <si>
-    <t>&lt;sqlalchemy.orm.state.InstanceState object at 0x7f0570ea1190&gt;</t>
-  </si>
-  <si>
-    <t>&lt;sqlalchemy.orm.state.InstanceState object at 0x7f0570ea1c10&gt;</t>
-  </si>
-  <si>
-    <t>&lt;sqlalchemy.orm.state.InstanceState object at 0x7f0570ea1970&gt;</t>
-  </si>
-  <si>
-    <t>&lt;sqlalchemy.orm.state.InstanceState object at 0x7f0570ea1c70&gt;</t>
-  </si>
-  <si>
-    <t>&lt;sqlalchemy.orm.state.InstanceState object at 0x7f0570ea1af0&gt;</t>
-  </si>
-  <si>
-    <t>&lt;sqlalchemy.orm.state.InstanceState object at 0x7f0570ea1580&gt;</t>
-  </si>
-  <si>
-    <t>&lt;sqlalchemy.orm.state.InstanceState object at 0x7f05504e21f0&gt;</t>
-  </si>
-  <si>
-    <t>&lt;sqlalchemy.orm.state.InstanceState object at 0x7f05504e2280&gt;</t>
-  </si>
-  <si>
-    <t>&lt;sqlalchemy.orm.state.InstanceState object at 0x7f05504e2310&gt;</t>
-  </si>
-  <si>
-    <t>&lt;sqlalchemy.orm.state.InstanceState object at 0x7f05504e23a0&gt;</t>
-  </si>
-  <si>
-    <t>&lt;sqlalchemy.orm.state.InstanceState object at 0x7f05504e2430&gt;</t>
-  </si>
-  <si>
-    <t>&lt;sqlalchemy.orm.state.InstanceState object at 0x7f05504e24c0&gt;</t>
-  </si>
-  <si>
-    <t>&lt;sqlalchemy.orm.state.InstanceState object at 0x7f05504e2550&gt;</t>
-  </si>
-  <si>
-    <t>&lt;sqlalchemy.orm.state.InstanceState object at 0x7f05504e25e0&gt;</t>
-  </si>
-  <si>
-    <t>&lt;sqlalchemy.orm.state.InstanceState object at 0x7f05504e2670&gt;</t>
+    <t>&lt;sqlalchemy.orm.state.InstanceState object at 0x7f8959ed6040&gt;</t>
+  </si>
+  <si>
+    <t>&lt;sqlalchemy.orm.state.InstanceState object at 0x7f8959ed62e0&gt;</t>
+  </si>
+  <si>
+    <t>&lt;sqlalchemy.orm.state.InstanceState object at 0x7f8959ed6100&gt;</t>
+  </si>
+  <si>
+    <t>&lt;sqlalchemy.orm.state.InstanceState object at 0x7f8959ed6070&gt;</t>
+  </si>
+  <si>
+    <t>&lt;sqlalchemy.orm.state.InstanceState object at 0x7f8959ed68b0&gt;</t>
+  </si>
+  <si>
+    <t>&lt;sqlalchemy.orm.state.InstanceState object at 0x7f8959ed69d0&gt;</t>
+  </si>
+  <si>
+    <t>&lt;sqlalchemy.orm.state.InstanceState object at 0x7f8959ed6ac0&gt;</t>
+  </si>
+  <si>
+    <t>&lt;sqlalchemy.orm.state.InstanceState object at 0x7f895a1588b0&gt;</t>
+  </si>
+  <si>
+    <t>&lt;sqlalchemy.orm.state.InstanceState object at 0x7f895a158af0&gt;</t>
+  </si>
+  <si>
+    <t>&lt;sqlalchemy.orm.state.InstanceState object at 0x7f895a158790&gt;</t>
+  </si>
+  <si>
+    <t>&lt;sqlalchemy.orm.state.InstanceState object at 0x7f895a158a90&gt;</t>
+  </si>
+  <si>
+    <t>&lt;sqlalchemy.orm.state.InstanceState object at 0x7f8942cd3700&gt;</t>
+  </si>
+  <si>
+    <t>&lt;sqlalchemy.orm.state.InstanceState object at 0x7f8942cd36a0&gt;</t>
+  </si>
+  <si>
+    <t>&lt;sqlalchemy.orm.state.InstanceState object at 0x7f8942cd35e0&gt;</t>
+  </si>
+  <si>
+    <t>&lt;sqlalchemy.orm.state.InstanceState object at 0x7f8942cd3640&gt;</t>
+  </si>
+  <si>
+    <t>&lt;sqlalchemy.orm.state.InstanceState object at 0x7f8942cd3610&gt;</t>
+  </si>
+  <si>
+    <t>&lt;sqlalchemy.orm.state.InstanceState object at 0x7f895812d580&gt;</t>
+  </si>
+  <si>
+    <t>&lt;sqlalchemy.orm.state.InstanceState object at 0x7f895812dee0&gt;</t>
+  </si>
+  <si>
+    <t>&lt;sqlalchemy.orm.state.InstanceState object at 0x7f89435155b0&gt;</t>
+  </si>
+  <si>
+    <t>&lt;sqlalchemy.orm.state.InstanceState object at 0x7f895a16d640&gt;</t>
+  </si>
+  <si>
+    <t>&lt;sqlalchemy.orm.state.InstanceState object at 0x7f895a16d280&gt;</t>
+  </si>
+  <si>
+    <t>&lt;sqlalchemy.orm.state.InstanceState object at 0x7f895a16dee0&gt;</t>
+  </si>
+  <si>
+    <t>&lt;sqlalchemy.orm.state.InstanceState object at 0x7f895a16df40&gt;</t>
+  </si>
+  <si>
+    <t>&lt;sqlalchemy.orm.state.InstanceState object at 0x7f895a17e280&gt;</t>
+  </si>
+  <si>
+    <t>&lt;sqlalchemy.orm.state.InstanceState object at 0x7f895a17ea90&gt;</t>
+  </si>
+  <si>
+    <t>&lt;sqlalchemy.orm.state.InstanceState object at 0x7f8942cd4550&gt;</t>
+  </si>
+  <si>
+    <t>&lt;sqlalchemy.orm.state.InstanceState object at 0x7f8942cd48e0&gt;</t>
+  </si>
+  <si>
+    <t>&lt;sqlalchemy.orm.state.InstanceState object at 0x7f8942cd4880&gt;</t>
+  </si>
+  <si>
+    <t>&lt;sqlalchemy.orm.state.InstanceState object at 0x7f8958125940&gt;</t>
+  </si>
+  <si>
+    <t>&lt;sqlalchemy.orm.state.InstanceState object at 0x7f8942cdcd60&gt;</t>
+  </si>
+  <si>
+    <t>&lt;sqlalchemy.orm.state.InstanceState object at 0x7f89599785e0&gt;</t>
+  </si>
+  <si>
+    <t>&lt;sqlalchemy.orm.state.InstanceState object at 0x7f8959971220&gt;</t>
+  </si>
+  <si>
+    <t>&lt;sqlalchemy.orm.state.InstanceState object at 0x7f895a1cc040&gt;</t>
+  </si>
+  <si>
+    <t>&lt;sqlalchemy.orm.state.InstanceState object at 0x7f895a1ccd90&gt;</t>
+  </si>
+  <si>
+    <t>&lt;sqlalchemy.orm.state.InstanceState object at 0x7f89434f5520&gt;</t>
+  </si>
+  <si>
+    <t>&lt;sqlalchemy.orm.state.InstanceState object at 0x7f89434f5ca0&gt;</t>
+  </si>
+  <si>
+    <t>&lt;sqlalchemy.orm.state.InstanceState object at 0x7f89434f5a30&gt;</t>
+  </si>
+  <si>
+    <t>&lt;sqlalchemy.orm.state.InstanceState object at 0x7f89434f5130&gt;</t>
+  </si>
+  <si>
+    <t>&lt;sqlalchemy.orm.state.InstanceState object at 0x7f895a140460&gt;</t>
+  </si>
+  <si>
+    <t>&lt;sqlalchemy.orm.state.InstanceState object at 0x7f895a1400a0&gt;</t>
+  </si>
+  <si>
+    <t>&lt;sqlalchemy.orm.state.InstanceState object at 0x7f8943576af0&gt;</t>
+  </si>
+  <si>
+    <t>&lt;sqlalchemy.orm.state.InstanceState object at 0x7f8943576dc0&gt;</t>
+  </si>
+  <si>
+    <t>&lt;sqlalchemy.orm.state.InstanceState object at 0x7f89435767f0&gt;</t>
+  </si>
+  <si>
+    <t>&lt;sqlalchemy.orm.state.InstanceState object at 0x7f89435760a0&gt;</t>
+  </si>
+  <si>
+    <t>&lt;sqlalchemy.orm.state.InstanceState object at 0x7f89434eaf70&gt;</t>
+  </si>
+  <si>
+    <t>&lt;sqlalchemy.orm.state.InstanceState object at 0x7f89434eae50&gt;</t>
+  </si>
+  <si>
+    <t>&lt;sqlalchemy.orm.state.InstanceState object at 0x7f89434ea2b0&gt;</t>
+  </si>
+  <si>
+    <t>&lt;sqlalchemy.orm.state.InstanceState object at 0x7f895a114a60&gt;</t>
+  </si>
+  <si>
+    <t>&lt;sqlalchemy.orm.state.InstanceState object at 0x7f895a114280&gt;</t>
+  </si>
+  <si>
+    <t>&lt;sqlalchemy.orm.state.InstanceState object at 0x7f8959ed6b20&gt;</t>
+  </si>
+  <si>
+    <t>&lt;sqlalchemy.orm.state.InstanceState object at 0x7f8959ed6be0&gt;</t>
+  </si>
+  <si>
+    <t>&lt;sqlalchemy.orm.state.InstanceState object at 0x7f8959ed6c70&gt;</t>
+  </si>
+  <si>
+    <t>&lt;sqlalchemy.orm.state.InstanceState object at 0x7f8959ed6d00&gt;</t>
+  </si>
+  <si>
+    <t>&lt;sqlalchemy.orm.state.InstanceState object at 0x7f8959ed6d90&gt;</t>
+  </si>
+  <si>
+    <t>&lt;sqlalchemy.orm.state.InstanceState object at 0x7f8959ed6e20&gt;</t>
+  </si>
+  <si>
+    <t>&lt;sqlalchemy.orm.state.InstanceState object at 0x7f8959ed6eb0&gt;</t>
+  </si>
+  <si>
+    <t>&lt;sqlalchemy.orm.state.InstanceState object at 0x7f8959ed6f40&gt;</t>
+  </si>
+  <si>
+    <t>&lt;sqlalchemy.orm.state.InstanceState object at 0x7f8959ed6fd0&gt;</t>
+  </si>
+  <si>
+    <t>&lt;sqlalchemy.orm.state.InstanceState object at 0x7f8959d460a0&gt;</t>
+  </si>
+  <si>
+    <t>&lt;sqlalchemy.orm.state.InstanceState object at 0x7f8959d46130&gt;</t>
+  </si>
+  <si>
+    <t>&lt;sqlalchemy.orm.state.InstanceState object at 0x7f8959d461c0&gt;</t>
+  </si>
+  <si>
+    <t>&lt;sqlalchemy.orm.state.InstanceState object at 0x7f8959d46250&gt;</t>
+  </si>
+  <si>
+    <t>&lt;sqlalchemy.orm.state.InstanceState object at 0x7f8959d462e0&gt;</t>
   </si>
   <si>
     <t>Configuration</t>
@@ -256,6 +262,21 @@
     <t>setup</t>
   </si>
   <si>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>cart</t>
+  </si>
+  <si>
+    <t>order</t>
+  </si>
+  <si>
+    <t>user</t>
+  </si>
+  <si>
+    <t>wishlist</t>
+  </si>
+  <si>
     <t>Insert</t>
   </si>
   <si>
@@ -265,21 +286,6 @@
     <t>Delete</t>
   </si>
   <si>
-    <t>admin</t>
-  </si>
-  <si>
-    <t>cart</t>
-  </si>
-  <si>
-    <t>order</t>
-  </si>
-  <si>
-    <t>user</t>
-  </si>
-  <si>
-    <t>wishlist</t>
-  </si>
-  <si>
     <t>19-May-2021 16:44:17</t>
   </si>
   <si>
@@ -389,6 +395,12 @@
   </si>
   <si>
     <t>20-May-2021 01:15:01</t>
+  </si>
+  <si>
+    <t>17-Jun-2021 19:04:19</t>
+  </si>
+  <si>
+    <t>17-Jun-2021 19:04:20</t>
   </si>
 </sst>
 </file>
@@ -746,7 +758,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H62"/>
+  <dimension ref="A1:H64"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -783,25 +795,25 @@
         <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E2" t="s">
-        <v>80</v>
-      </c>
-      <c r="F2" t="s">
-        <v>83</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
+        <v>82</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2" t="s">
+        <v>87</v>
       </c>
       <c r="H2" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -809,25 +821,25 @@
         <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E3" t="s">
-        <v>80</v>
-      </c>
-      <c r="F3" t="s">
-        <v>83</v>
-      </c>
-      <c r="G3">
+        <v>82</v>
+      </c>
+      <c r="F3">
         <v>2</v>
       </c>
+      <c r="G3" t="s">
+        <v>87</v>
+      </c>
       <c r="H3" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -835,25 +847,25 @@
         <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E4" t="s">
-        <v>81</v>
-      </c>
-      <c r="F4" t="s">
-        <v>83</v>
-      </c>
-      <c r="G4">
+        <v>82</v>
+      </c>
+      <c r="F4">
         <v>3</v>
       </c>
+      <c r="G4" t="s">
+        <v>88</v>
+      </c>
       <c r="H4" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -861,25 +873,25 @@
         <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C5">
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E5" t="s">
-        <v>81</v>
-      </c>
-      <c r="F5" t="s">
-        <v>84</v>
-      </c>
-      <c r="G5">
+        <v>83</v>
+      </c>
+      <c r="F5">
         <v>4</v>
       </c>
+      <c r="G5" t="s">
+        <v>88</v>
+      </c>
       <c r="H5" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -887,25 +899,25 @@
         <v>12</v>
       </c>
       <c r="B6" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="C6">
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E6" t="s">
-        <v>81</v>
-      </c>
-      <c r="F6" t="s">
-        <v>84</v>
-      </c>
-      <c r="G6">
+        <v>83</v>
+      </c>
+      <c r="F6">
         <v>5</v>
       </c>
+      <c r="G6" t="s">
+        <v>88</v>
+      </c>
       <c r="H6" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -913,25 +925,25 @@
         <v>13</v>
       </c>
       <c r="B7" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C7">
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E7" t="s">
-        <v>80</v>
-      </c>
-      <c r="F7" t="s">
-        <v>85</v>
-      </c>
-      <c r="G7">
+        <v>84</v>
+      </c>
+      <c r="F7">
         <v>6</v>
       </c>
+      <c r="G7" t="s">
+        <v>87</v>
+      </c>
       <c r="H7" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -939,25 +951,25 @@
         <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C8">
         <v>1</v>
       </c>
       <c r="D8" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E8" t="s">
-        <v>80</v>
-      </c>
-      <c r="F8" t="s">
-        <v>85</v>
-      </c>
-      <c r="G8">
+        <v>84</v>
+      </c>
+      <c r="F8">
         <v>7</v>
       </c>
+      <c r="G8" t="s">
+        <v>87</v>
+      </c>
       <c r="H8" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -965,25 +977,25 @@
         <v>15</v>
       </c>
       <c r="B9" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C9">
         <v>1</v>
       </c>
       <c r="D9" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E9" t="s">
-        <v>82</v>
-      </c>
-      <c r="F9" t="s">
-        <v>84</v>
-      </c>
-      <c r="G9">
+        <v>83</v>
+      </c>
+      <c r="F9">
         <v>8</v>
       </c>
+      <c r="G9" t="s">
+        <v>89</v>
+      </c>
       <c r="H9" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -991,25 +1003,25 @@
         <v>16</v>
       </c>
       <c r="B10" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C10">
         <v>1</v>
       </c>
       <c r="D10" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E10" t="s">
-        <v>80</v>
-      </c>
-      <c r="F10" t="s">
-        <v>86</v>
-      </c>
-      <c r="G10">
+        <v>85</v>
+      </c>
+      <c r="F10">
         <v>9</v>
       </c>
+      <c r="G10" t="s">
+        <v>87</v>
+      </c>
       <c r="H10" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -1017,25 +1029,25 @@
         <v>17</v>
       </c>
       <c r="B11" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="C11">
         <v>1</v>
       </c>
       <c r="D11" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E11" t="s">
-        <v>80</v>
-      </c>
-      <c r="F11" t="s">
-        <v>84</v>
-      </c>
-      <c r="G11">
+        <v>83</v>
+      </c>
+      <c r="F11">
         <v>10</v>
       </c>
+      <c r="G11" t="s">
+        <v>87</v>
+      </c>
       <c r="H11" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -1043,25 +1055,25 @@
         <v>18</v>
       </c>
       <c r="B12" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C12">
         <v>1</v>
       </c>
       <c r="D12" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E12" t="s">
-        <v>80</v>
-      </c>
-      <c r="F12" t="s">
-        <v>84</v>
-      </c>
-      <c r="G12">
+        <v>83</v>
+      </c>
+      <c r="F12">
         <v>11</v>
       </c>
+      <c r="G12" t="s">
+        <v>87</v>
+      </c>
       <c r="H12" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -1069,25 +1081,25 @@
         <v>19</v>
       </c>
       <c r="B13" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="C13">
         <v>1</v>
       </c>
       <c r="D13" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E13" t="s">
-        <v>81</v>
-      </c>
-      <c r="F13" t="s">
-        <v>84</v>
-      </c>
-      <c r="G13">
+        <v>83</v>
+      </c>
+      <c r="F13">
         <v>12</v>
       </c>
+      <c r="G13" t="s">
+        <v>88</v>
+      </c>
       <c r="H13" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -1095,25 +1107,25 @@
         <v>20</v>
       </c>
       <c r="B14" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C14">
         <v>1</v>
       </c>
       <c r="D14" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E14" t="s">
-        <v>80</v>
-      </c>
-      <c r="F14" t="s">
-        <v>84</v>
-      </c>
-      <c r="G14">
+        <v>83</v>
+      </c>
+      <c r="F14">
         <v>13</v>
       </c>
+      <c r="G14" t="s">
+        <v>87</v>
+      </c>
       <c r="H14" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="15" spans="1:8">
@@ -1121,25 +1133,25 @@
         <v>21</v>
       </c>
       <c r="B15" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="C15">
         <v>1</v>
       </c>
       <c r="D15" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E15" t="s">
-        <v>81</v>
-      </c>
-      <c r="F15" t="s">
-        <v>84</v>
-      </c>
-      <c r="G15">
+        <v>83</v>
+      </c>
+      <c r="F15">
         <v>14</v>
       </c>
+      <c r="G15" t="s">
+        <v>88</v>
+      </c>
       <c r="H15" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="16" spans="1:8">
@@ -1147,25 +1159,25 @@
         <v>22</v>
       </c>
       <c r="B16" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C16">
         <v>1</v>
       </c>
       <c r="D16" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E16" t="s">
-        <v>81</v>
-      </c>
-      <c r="F16" t="s">
-        <v>84</v>
-      </c>
-      <c r="G16">
+        <v>83</v>
+      </c>
+      <c r="F16">
         <v>15</v>
       </c>
+      <c r="G16" t="s">
+        <v>88</v>
+      </c>
       <c r="H16" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
     </row>
     <row r="17" spans="1:8">
@@ -1173,25 +1185,25 @@
         <v>23</v>
       </c>
       <c r="B17" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="C17">
         <v>1</v>
       </c>
       <c r="D17" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E17" t="s">
-        <v>81</v>
-      </c>
-      <c r="F17" t="s">
-        <v>84</v>
-      </c>
-      <c r="G17">
+        <v>83</v>
+      </c>
+      <c r="F17">
         <v>16</v>
       </c>
+      <c r="G17" t="s">
+        <v>88</v>
+      </c>
       <c r="H17" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
     </row>
     <row r="18" spans="1:8">
@@ -1199,25 +1211,25 @@
         <v>24</v>
       </c>
       <c r="B18" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C18">
         <v>1</v>
       </c>
       <c r="D18" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E18" t="s">
-        <v>81</v>
-      </c>
-      <c r="F18" t="s">
-        <v>84</v>
-      </c>
-      <c r="G18">
+        <v>83</v>
+      </c>
+      <c r="F18">
         <v>17</v>
       </c>
+      <c r="G18" t="s">
+        <v>88</v>
+      </c>
       <c r="H18" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
     </row>
     <row r="19" spans="1:8">
@@ -1225,25 +1237,25 @@
         <v>25</v>
       </c>
       <c r="B19" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="C19">
         <v>1</v>
       </c>
       <c r="D19" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E19" t="s">
-        <v>81</v>
-      </c>
-      <c r="F19" t="s">
-        <v>84</v>
-      </c>
-      <c r="G19">
+        <v>83</v>
+      </c>
+      <c r="F19">
         <v>18</v>
       </c>
+      <c r="G19" t="s">
+        <v>88</v>
+      </c>
       <c r="H19" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
     </row>
     <row r="20" spans="1:8">
@@ -1251,25 +1263,25 @@
         <v>26</v>
       </c>
       <c r="B20" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C20">
         <v>1</v>
       </c>
       <c r="D20" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E20" t="s">
-        <v>81</v>
-      </c>
-      <c r="F20" t="s">
-        <v>84</v>
-      </c>
-      <c r="G20">
+        <v>83</v>
+      </c>
+      <c r="F20">
         <v>19</v>
       </c>
+      <c r="G20" t="s">
+        <v>88</v>
+      </c>
       <c r="H20" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="21" spans="1:8">
@@ -1277,25 +1289,25 @@
         <v>27</v>
       </c>
       <c r="B21" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="C21">
         <v>1</v>
       </c>
       <c r="D21" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E21" t="s">
-        <v>81</v>
-      </c>
-      <c r="F21" t="s">
-        <v>84</v>
-      </c>
-      <c r="G21">
+        <v>83</v>
+      </c>
+      <c r="F21">
         <v>20</v>
       </c>
+      <c r="G21" t="s">
+        <v>88</v>
+      </c>
       <c r="H21" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="22" spans="1:8">
@@ -1303,25 +1315,25 @@
         <v>28</v>
       </c>
       <c r="B22" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="C22">
         <v>1</v>
       </c>
       <c r="D22" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E22" t="s">
-        <v>80</v>
-      </c>
-      <c r="F22" t="s">
-        <v>86</v>
-      </c>
-      <c r="G22">
+        <v>85</v>
+      </c>
+      <c r="F22">
         <v>21</v>
       </c>
+      <c r="G22" t="s">
+        <v>87</v>
+      </c>
       <c r="H22" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
     </row>
     <row r="23" spans="1:8">
@@ -1329,25 +1341,25 @@
         <v>29</v>
       </c>
       <c r="B23" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C23">
         <v>1</v>
       </c>
       <c r="D23" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E23" t="s">
-        <v>80</v>
-      </c>
-      <c r="F23" t="s">
-        <v>86</v>
-      </c>
-      <c r="G23">
+        <v>85</v>
+      </c>
+      <c r="F23">
         <v>22</v>
       </c>
+      <c r="G23" t="s">
+        <v>87</v>
+      </c>
       <c r="H23" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
     </row>
     <row r="24" spans="1:8">
@@ -1355,25 +1367,25 @@
         <v>30</v>
       </c>
       <c r="B24" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C24">
         <v>1</v>
       </c>
       <c r="D24" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E24" t="s">
-        <v>80</v>
-      </c>
-      <c r="F24" t="s">
-        <v>85</v>
-      </c>
-      <c r="G24">
+        <v>84</v>
+      </c>
+      <c r="F24">
         <v>23</v>
       </c>
+      <c r="G24" t="s">
+        <v>87</v>
+      </c>
       <c r="H24" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
     </row>
     <row r="25" spans="1:8">
@@ -1381,25 +1393,25 @@
         <v>31</v>
       </c>
       <c r="B25" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C25">
         <v>1</v>
       </c>
       <c r="D25" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E25" t="s">
-        <v>80</v>
-      </c>
-      <c r="F25" t="s">
-        <v>85</v>
-      </c>
-      <c r="G25">
+        <v>84</v>
+      </c>
+      <c r="F25">
         <v>24</v>
       </c>
+      <c r="G25" t="s">
+        <v>87</v>
+      </c>
       <c r="H25" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
     </row>
     <row r="26" spans="1:8">
@@ -1407,25 +1419,25 @@
         <v>32</v>
       </c>
       <c r="B26" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C26">
         <v>1</v>
       </c>
       <c r="D26" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E26" t="s">
-        <v>80</v>
-      </c>
-      <c r="F26" t="s">
-        <v>85</v>
-      </c>
-      <c r="G26">
+        <v>84</v>
+      </c>
+      <c r="F26">
         <v>25</v>
       </c>
+      <c r="G26" t="s">
+        <v>87</v>
+      </c>
       <c r="H26" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
     </row>
     <row r="27" spans="1:8">
@@ -1433,25 +1445,25 @@
         <v>33</v>
       </c>
       <c r="B27" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="C27">
         <v>1</v>
       </c>
       <c r="D27" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E27" t="s">
-        <v>81</v>
-      </c>
-      <c r="F27" t="s">
-        <v>84</v>
-      </c>
-      <c r="G27">
+        <v>83</v>
+      </c>
+      <c r="F27">
         <v>26</v>
       </c>
+      <c r="G27" t="s">
+        <v>88</v>
+      </c>
       <c r="H27" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
     </row>
     <row r="28" spans="1:8">
@@ -1459,25 +1471,25 @@
         <v>34</v>
       </c>
       <c r="B28" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C28">
         <v>1</v>
       </c>
       <c r="D28" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E28" t="s">
-        <v>82</v>
-      </c>
-      <c r="F28" t="s">
-        <v>84</v>
-      </c>
-      <c r="G28">
+        <v>83</v>
+      </c>
+      <c r="F28">
         <v>27</v>
       </c>
+      <c r="G28" t="s">
+        <v>89</v>
+      </c>
       <c r="H28" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
     </row>
     <row r="29" spans="1:8">
@@ -1485,25 +1497,25 @@
         <v>35</v>
       </c>
       <c r="B29" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C29">
         <v>1</v>
       </c>
       <c r="D29" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E29" t="s">
-        <v>82</v>
-      </c>
-      <c r="F29" t="s">
-        <v>84</v>
-      </c>
-      <c r="G29">
+        <v>83</v>
+      </c>
+      <c r="F29">
         <v>28</v>
       </c>
+      <c r="G29" t="s">
+        <v>89</v>
+      </c>
       <c r="H29" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
     </row>
     <row r="30" spans="1:8">
@@ -1511,25 +1523,25 @@
         <v>36</v>
       </c>
       <c r="B30" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C30">
         <v>1</v>
       </c>
       <c r="D30" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E30" t="s">
-        <v>81</v>
-      </c>
-      <c r="F30" t="s">
-        <v>85</v>
-      </c>
-      <c r="G30">
+        <v>84</v>
+      </c>
+      <c r="F30">
         <v>29</v>
       </c>
+      <c r="G30" t="s">
+        <v>88</v>
+      </c>
       <c r="H30" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
     </row>
     <row r="31" spans="1:8">
@@ -1537,25 +1549,25 @@
         <v>37</v>
       </c>
       <c r="B31" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C31">
         <v>1</v>
       </c>
       <c r="D31" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E31" t="s">
-        <v>81</v>
-      </c>
-      <c r="F31" t="s">
-        <v>85</v>
-      </c>
-      <c r="G31">
+        <v>84</v>
+      </c>
+      <c r="F31">
         <v>30</v>
       </c>
+      <c r="G31" t="s">
+        <v>88</v>
+      </c>
       <c r="H31" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
     </row>
     <row r="32" spans="1:8">
@@ -1563,25 +1575,25 @@
         <v>38</v>
       </c>
       <c r="B32" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C32">
         <v>1</v>
       </c>
       <c r="D32" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E32" t="s">
-        <v>81</v>
-      </c>
-      <c r="F32" t="s">
-        <v>85</v>
-      </c>
-      <c r="G32">
+        <v>84</v>
+      </c>
+      <c r="F32">
         <v>31</v>
       </c>
+      <c r="G32" t="s">
+        <v>88</v>
+      </c>
       <c r="H32" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="33" spans="1:8">
@@ -1589,25 +1601,25 @@
         <v>39</v>
       </c>
       <c r="B33" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C33">
         <v>1</v>
       </c>
       <c r="D33" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E33" t="s">
-        <v>81</v>
-      </c>
-      <c r="F33" t="s">
-        <v>85</v>
-      </c>
-      <c r="G33">
+        <v>84</v>
+      </c>
+      <c r="F33">
         <v>32</v>
       </c>
+      <c r="G33" t="s">
+        <v>88</v>
+      </c>
       <c r="H33" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row r="34" spans="1:8">
@@ -1615,25 +1627,25 @@
         <v>40</v>
       </c>
       <c r="B34" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C34">
         <v>1</v>
       </c>
       <c r="D34" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E34" t="s">
-        <v>80</v>
-      </c>
-      <c r="F34" t="s">
-        <v>86</v>
-      </c>
-      <c r="G34">
+        <v>85</v>
+      </c>
+      <c r="F34">
         <v>33</v>
       </c>
+      <c r="G34" t="s">
+        <v>87</v>
+      </c>
       <c r="H34" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
     </row>
     <row r="35" spans="1:8">
@@ -1641,25 +1653,25 @@
         <v>41</v>
       </c>
       <c r="B35" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="C35">
         <v>1</v>
       </c>
       <c r="D35" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E35" t="s">
-        <v>80</v>
-      </c>
-      <c r="F35" t="s">
-        <v>84</v>
-      </c>
-      <c r="G35">
+        <v>83</v>
+      </c>
+      <c r="F35">
         <v>34</v>
       </c>
+      <c r="G35" t="s">
+        <v>87</v>
+      </c>
       <c r="H35" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
     </row>
     <row r="36" spans="1:8">
@@ -1667,25 +1679,25 @@
         <v>42</v>
       </c>
       <c r="B36" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C36">
         <v>1</v>
       </c>
       <c r="D36" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E36" t="s">
-        <v>80</v>
-      </c>
-      <c r="F36" t="s">
-        <v>84</v>
-      </c>
-      <c r="G36">
+        <v>83</v>
+      </c>
+      <c r="F36">
         <v>35</v>
       </c>
+      <c r="G36" t="s">
+        <v>87</v>
+      </c>
       <c r="H36" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
     </row>
     <row r="37" spans="1:8">
@@ -1693,25 +1705,25 @@
         <v>43</v>
       </c>
       <c r="B37" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="C37">
         <v>1</v>
       </c>
       <c r="D37" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E37" t="s">
-        <v>81</v>
-      </c>
-      <c r="F37" t="s">
-        <v>84</v>
-      </c>
-      <c r="G37">
+        <v>83</v>
+      </c>
+      <c r="F37">
         <v>36</v>
       </c>
+      <c r="G37" t="s">
+        <v>88</v>
+      </c>
       <c r="H37" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
     </row>
     <row r="38" spans="1:8">
@@ -1719,25 +1731,25 @@
         <v>44</v>
       </c>
       <c r="B38" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C38">
         <v>1</v>
       </c>
       <c r="D38" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E38" t="s">
-        <v>80</v>
-      </c>
-      <c r="F38" t="s">
-        <v>84</v>
-      </c>
-      <c r="G38">
+        <v>83</v>
+      </c>
+      <c r="F38">
         <v>37</v>
       </c>
+      <c r="G38" t="s">
+        <v>87</v>
+      </c>
       <c r="H38" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="39" spans="1:8">
@@ -1745,25 +1757,25 @@
         <v>45</v>
       </c>
       <c r="B39" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="C39">
         <v>1</v>
       </c>
       <c r="D39" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E39" t="s">
-        <v>81</v>
-      </c>
-      <c r="F39" t="s">
-        <v>84</v>
-      </c>
-      <c r="G39">
+        <v>83</v>
+      </c>
+      <c r="F39">
         <v>38</v>
       </c>
+      <c r="G39" t="s">
+        <v>88</v>
+      </c>
       <c r="H39" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="40" spans="1:8">
@@ -1771,25 +1783,25 @@
         <v>46</v>
       </c>
       <c r="B40" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C40">
         <v>1</v>
       </c>
       <c r="D40" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E40" t="s">
-        <v>81</v>
-      </c>
-      <c r="F40" t="s">
-        <v>84</v>
-      </c>
-      <c r="G40">
+        <v>83</v>
+      </c>
+      <c r="F40">
         <v>39</v>
       </c>
+      <c r="G40" t="s">
+        <v>88</v>
+      </c>
       <c r="H40" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="41" spans="1:8">
@@ -1797,25 +1809,25 @@
         <v>47</v>
       </c>
       <c r="B41" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="C41">
         <v>1</v>
       </c>
       <c r="D41" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E41" t="s">
-        <v>81</v>
-      </c>
-      <c r="F41" t="s">
-        <v>84</v>
-      </c>
-      <c r="G41">
+        <v>83</v>
+      </c>
+      <c r="F41">
         <v>40</v>
       </c>
+      <c r="G41" t="s">
+        <v>88</v>
+      </c>
       <c r="H41" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="42" spans="1:8">
@@ -1823,25 +1835,25 @@
         <v>48</v>
       </c>
       <c r="B42" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C42">
         <v>1</v>
       </c>
       <c r="D42" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E42" t="s">
-        <v>81</v>
-      </c>
-      <c r="F42" t="s">
-        <v>84</v>
-      </c>
-      <c r="G42">
+        <v>83</v>
+      </c>
+      <c r="F42">
         <v>41</v>
       </c>
+      <c r="G42" t="s">
+        <v>88</v>
+      </c>
       <c r="H42" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
     </row>
     <row r="43" spans="1:8">
@@ -1849,25 +1861,25 @@
         <v>49</v>
       </c>
       <c r="B43" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="C43">
         <v>1</v>
       </c>
       <c r="D43" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E43" t="s">
-        <v>81</v>
-      </c>
-      <c r="F43" t="s">
-        <v>84</v>
-      </c>
-      <c r="G43">
+        <v>83</v>
+      </c>
+      <c r="F43">
         <v>42</v>
       </c>
+      <c r="G43" t="s">
+        <v>88</v>
+      </c>
       <c r="H43" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
     </row>
     <row r="44" spans="1:8">
@@ -1875,25 +1887,25 @@
         <v>50</v>
       </c>
       <c r="B44" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C44">
         <v>1</v>
       </c>
       <c r="D44" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E44" t="s">
-        <v>81</v>
-      </c>
-      <c r="F44" t="s">
-        <v>84</v>
-      </c>
-      <c r="G44">
+        <v>83</v>
+      </c>
+      <c r="F44">
         <v>43</v>
       </c>
+      <c r="G44" t="s">
+        <v>88</v>
+      </c>
       <c r="H44" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
     </row>
     <row r="45" spans="1:8">
@@ -1901,25 +1913,25 @@
         <v>51</v>
       </c>
       <c r="B45" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="C45">
         <v>1</v>
       </c>
       <c r="D45" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E45" t="s">
-        <v>81</v>
-      </c>
-      <c r="F45" t="s">
-        <v>84</v>
-      </c>
-      <c r="G45">
+        <v>83</v>
+      </c>
+      <c r="F45">
         <v>44</v>
       </c>
+      <c r="G45" t="s">
+        <v>88</v>
+      </c>
       <c r="H45" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
     </row>
     <row r="46" spans="1:8">
@@ -1927,25 +1939,25 @@
         <v>52</v>
       </c>
       <c r="B46" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="C46">
         <v>1</v>
       </c>
       <c r="D46" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E46" t="s">
-        <v>80</v>
-      </c>
-      <c r="F46" t="s">
-        <v>86</v>
-      </c>
-      <c r="G46">
+        <v>85</v>
+      </c>
+      <c r="F46">
         <v>45</v>
       </c>
+      <c r="G46" t="s">
+        <v>87</v>
+      </c>
       <c r="H46" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
     </row>
     <row r="47" spans="1:8">
@@ -1953,25 +1965,25 @@
         <v>53</v>
       </c>
       <c r="B47" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C47">
         <v>1</v>
       </c>
       <c r="D47" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E47" t="s">
-        <v>80</v>
-      </c>
-      <c r="F47" t="s">
-        <v>86</v>
-      </c>
-      <c r="G47">
+        <v>85</v>
+      </c>
+      <c r="F47">
         <v>46</v>
       </c>
+      <c r="G47" t="s">
+        <v>87</v>
+      </c>
       <c r="H47" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
     </row>
     <row r="48" spans="1:8">
@@ -1979,25 +1991,25 @@
         <v>54</v>
       </c>
       <c r="B48" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C48">
         <v>1</v>
       </c>
       <c r="D48" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E48" t="s">
-        <v>80</v>
-      </c>
-      <c r="F48" t="s">
-        <v>85</v>
-      </c>
-      <c r="G48">
+        <v>84</v>
+      </c>
+      <c r="F48">
         <v>47</v>
       </c>
+      <c r="G48" t="s">
+        <v>87</v>
+      </c>
       <c r="H48" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
     </row>
     <row r="49" spans="1:8">
@@ -2005,25 +2017,25 @@
         <v>55</v>
       </c>
       <c r="B49" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C49">
         <v>1</v>
       </c>
       <c r="D49" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E49" t="s">
-        <v>80</v>
-      </c>
-      <c r="F49" t="s">
-        <v>85</v>
-      </c>
-      <c r="G49">
+        <v>84</v>
+      </c>
+      <c r="F49">
         <v>48</v>
       </c>
+      <c r="G49" t="s">
+        <v>87</v>
+      </c>
       <c r="H49" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
     </row>
     <row r="50" spans="1:8">
@@ -2031,25 +2043,25 @@
         <v>56</v>
       </c>
       <c r="B50" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C50">
         <v>1</v>
       </c>
       <c r="D50" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E50" t="s">
-        <v>80</v>
-      </c>
-      <c r="F50" t="s">
-        <v>85</v>
-      </c>
-      <c r="G50">
+        <v>84</v>
+      </c>
+      <c r="F50">
         <v>49</v>
       </c>
+      <c r="G50" t="s">
+        <v>87</v>
+      </c>
       <c r="H50" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
     </row>
     <row r="51" spans="1:8">
@@ -2057,25 +2069,25 @@
         <v>57</v>
       </c>
       <c r="B51" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="C51">
         <v>1</v>
       </c>
       <c r="D51" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E51" t="s">
-        <v>81</v>
-      </c>
-      <c r="F51" t="s">
-        <v>84</v>
-      </c>
-      <c r="G51">
+        <v>83</v>
+      </c>
+      <c r="F51">
         <v>50</v>
       </c>
+      <c r="G51" t="s">
+        <v>88</v>
+      </c>
       <c r="H51" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
     </row>
     <row r="52" spans="1:8">
@@ -2083,25 +2095,25 @@
         <v>58</v>
       </c>
       <c r="B52" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C52">
         <v>1</v>
       </c>
       <c r="D52" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E52" t="s">
-        <v>82</v>
-      </c>
-      <c r="F52" t="s">
-        <v>84</v>
-      </c>
-      <c r="G52">
+        <v>83</v>
+      </c>
+      <c r="F52">
         <v>51</v>
       </c>
+      <c r="G52" t="s">
+        <v>89</v>
+      </c>
       <c r="H52" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
     </row>
     <row r="53" spans="1:8">
@@ -2109,25 +2121,25 @@
         <v>59</v>
       </c>
       <c r="B53" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C53">
         <v>1</v>
       </c>
       <c r="D53" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E53" t="s">
-        <v>82</v>
-      </c>
-      <c r="F53" t="s">
-        <v>84</v>
-      </c>
-      <c r="G53">
+        <v>83</v>
+      </c>
+      <c r="F53">
         <v>52</v>
       </c>
+      <c r="G53" t="s">
+        <v>89</v>
+      </c>
       <c r="H53" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
     </row>
     <row r="54" spans="1:8">
@@ -2135,25 +2147,25 @@
         <v>60</v>
       </c>
       <c r="B54" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C54">
         <v>1</v>
       </c>
       <c r="D54" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E54" t="s">
-        <v>81</v>
-      </c>
-      <c r="F54" t="s">
-        <v>85</v>
-      </c>
-      <c r="G54">
+        <v>84</v>
+      </c>
+      <c r="F54">
         <v>53</v>
       </c>
+      <c r="G54" t="s">
+        <v>88</v>
+      </c>
       <c r="H54" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
     </row>
     <row r="55" spans="1:8">
@@ -2161,25 +2173,25 @@
         <v>61</v>
       </c>
       <c r="B55" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C55">
         <v>1</v>
       </c>
       <c r="D55" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E55" t="s">
-        <v>81</v>
-      </c>
-      <c r="F55" t="s">
-        <v>85</v>
-      </c>
-      <c r="G55">
+        <v>84</v>
+      </c>
+      <c r="F55">
         <v>54</v>
       </c>
+      <c r="G55" t="s">
+        <v>88</v>
+      </c>
       <c r="H55" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
     </row>
     <row r="56" spans="1:8">
@@ -2187,25 +2199,25 @@
         <v>62</v>
       </c>
       <c r="B56" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C56">
         <v>1</v>
       </c>
       <c r="D56" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E56" t="s">
-        <v>81</v>
-      </c>
-      <c r="F56" t="s">
-        <v>85</v>
-      </c>
-      <c r="G56">
+        <v>84</v>
+      </c>
+      <c r="F56">
         <v>55</v>
       </c>
+      <c r="G56" t="s">
+        <v>88</v>
+      </c>
       <c r="H56" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
     </row>
     <row r="57" spans="1:8">
@@ -2213,25 +2225,25 @@
         <v>63</v>
       </c>
       <c r="B57" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C57">
         <v>1</v>
       </c>
       <c r="D57" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E57" t="s">
-        <v>81</v>
-      </c>
-      <c r="F57" t="s">
-        <v>85</v>
-      </c>
-      <c r="G57">
+        <v>84</v>
+      </c>
+      <c r="F57">
         <v>56</v>
       </c>
+      <c r="G57" t="s">
+        <v>88</v>
+      </c>
       <c r="H57" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
     </row>
     <row r="58" spans="1:8">
@@ -2239,25 +2251,25 @@
         <v>64</v>
       </c>
       <c r="B58" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C58">
         <v>1</v>
       </c>
       <c r="D58" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E58" t="s">
-        <v>80</v>
-      </c>
-      <c r="F58" t="s">
-        <v>87</v>
-      </c>
-      <c r="G58">
+        <v>86</v>
+      </c>
+      <c r="F58">
         <v>57</v>
       </c>
+      <c r="G58" t="s">
+        <v>87</v>
+      </c>
       <c r="H58" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
     </row>
     <row r="59" spans="1:8">
@@ -2265,25 +2277,25 @@
         <v>65</v>
       </c>
       <c r="B59" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C59">
         <v>1</v>
       </c>
       <c r="D59" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E59" t="s">
-        <v>80</v>
-      </c>
-      <c r="F59" t="s">
-        <v>87</v>
-      </c>
-      <c r="G59">
+        <v>86</v>
+      </c>
+      <c r="F59">
         <v>58</v>
       </c>
+      <c r="G59" t="s">
+        <v>87</v>
+      </c>
       <c r="H59" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
     </row>
     <row r="60" spans="1:8">
@@ -2291,25 +2303,25 @@
         <v>66</v>
       </c>
       <c r="B60" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C60">
         <v>1</v>
       </c>
       <c r="D60" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E60" t="s">
-        <v>82</v>
-      </c>
-      <c r="F60" t="s">
-        <v>87</v>
-      </c>
-      <c r="G60">
+        <v>86</v>
+      </c>
+      <c r="F60">
         <v>59</v>
       </c>
+      <c r="G60" t="s">
+        <v>89</v>
+      </c>
       <c r="H60" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
     </row>
     <row r="61" spans="1:8">
@@ -2317,25 +2329,25 @@
         <v>67</v>
       </c>
       <c r="B61" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C61">
         <v>1</v>
       </c>
       <c r="D61" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E61" t="s">
-        <v>80</v>
-      </c>
-      <c r="F61" t="s">
-        <v>87</v>
-      </c>
-      <c r="G61">
+        <v>86</v>
+      </c>
+      <c r="F61">
         <v>60</v>
       </c>
+      <c r="G61" t="s">
+        <v>87</v>
+      </c>
       <c r="H61" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
     </row>
     <row r="62" spans="1:8">
@@ -2343,25 +2355,77 @@
         <v>68</v>
       </c>
       <c r="B62" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C62">
         <v>1</v>
       </c>
       <c r="D62" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E62" t="s">
-        <v>80</v>
-      </c>
-      <c r="F62" t="s">
-        <v>87</v>
-      </c>
-      <c r="G62">
+        <v>86</v>
+      </c>
+      <c r="F62">
         <v>61</v>
       </c>
+      <c r="G62" t="s">
+        <v>87</v>
+      </c>
       <c r="H62" t="s">
-        <v>124</v>
+        <v>126</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8">
+      <c r="A63" t="s">
+        <v>69</v>
+      </c>
+      <c r="B63" t="s">
+        <v>73</v>
+      </c>
+      <c r="C63">
+        <v>1</v>
+      </c>
+      <c r="D63" t="s">
+        <v>81</v>
+      </c>
+      <c r="E63" t="s">
+        <v>83</v>
+      </c>
+      <c r="F63">
+        <v>62</v>
+      </c>
+      <c r="G63" t="s">
+        <v>87</v>
+      </c>
+      <c r="H63" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8">
+      <c r="A64" t="s">
+        <v>70</v>
+      </c>
+      <c r="B64" t="s">
+        <v>74</v>
+      </c>
+      <c r="C64">
+        <v>1</v>
+      </c>
+      <c r="D64" t="s">
+        <v>81</v>
+      </c>
+      <c r="E64" t="s">
+        <v>83</v>
+      </c>
+      <c r="F64">
+        <v>63</v>
+      </c>
+      <c r="G64" t="s">
+        <v>88</v>
+      </c>
+      <c r="H64" t="s">
+        <v>128</v>
       </c>
     </row>
   </sheetData>

</xml_diff>